<commit_message>
Reformatted both documents with feedback
Includes internal vs external due dates, and complexity of each Work Item. Replaced term "task" with "work item"
</commit_message>
<xml_diff>
--- a/Scrum Artifacts/Product Backlog.xlsx
+++ b/Scrum Artifacts/Product Backlog.xlsx
@@ -11,33 +11,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>No.</t>
   </si>
   <si>
-    <t>Task</t>
+    <t>Work Item</t>
   </si>
   <si>
     <t>Effort (Hours)</t>
   </si>
   <si>
-    <t>Due Date</t>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t>Internal Due Date</t>
+  </si>
+  <si>
+    <t>External Due Date</t>
   </si>
   <si>
     <t>Project Proposal</t>
   </si>
   <si>
-    <t>9/11/2023/ASAP</t>
+    <t xml:space="preserve">High </t>
+  </si>
+  <si>
+    <t>Past Due - ASAP</t>
   </si>
   <si>
     <t>Coding Environment Setup</t>
   </si>
   <si>
+    <t xml:space="preserve">Low </t>
+  </si>
+  <si>
     <t>BRD</t>
   </si>
   <si>
     <t>Team Review 1</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
   <si>
     <t>Milestone 1</t>
@@ -59,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm d"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -71,12 +86,8 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,12 +100,6 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -102,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -112,13 +117,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -357,19 +359,31 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>15.0</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3">
+        <v>45180.0</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -377,12 +391,18 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2">
         <v>8.0</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>45193.0</v>
+      </c>
+      <c r="F3" s="3">
         <v>45194.0</v>
       </c>
     </row>
@@ -391,12 +411,18 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>30.0</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45195.0</v>
+      </c>
+      <c r="F4" s="3">
         <v>45196.0</v>
       </c>
     </row>
@@ -405,12 +431,18 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
         <v>20.0</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3">
+        <v>45195.0</v>
+      </c>
+      <c r="F5" s="3">
         <v>45196.0</v>
       </c>
     </row>
@@ -419,12 +451,18 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2">
         <v>60.0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>45237.0</v>
+      </c>
+      <c r="F6" s="3">
         <v>45238.0</v>
       </c>
     </row>
@@ -433,12 +471,18 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2">
         <v>20.0</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3">
+        <v>45237.0</v>
+      </c>
+      <c r="F7" s="3">
         <v>45238.0</v>
       </c>
     </row>
@@ -447,12 +491,18 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2">
         <v>60.0</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3">
+        <v>45270.0</v>
+      </c>
+      <c r="F8" s="3">
         <v>45271.0</v>
       </c>
     </row>
@@ -461,12 +511,18 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2">
         <v>20.0</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3">
+        <v>45270.0</v>
+      </c>
+      <c r="F9" s="3">
         <v>45271.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Project Backlog @ Backlog Grooming
</commit_message>
<xml_diff>
--- a/Scrum Artifacts/Product Backlog.xlsx
+++ b/Scrum Artifacts/Product Backlog.xlsx
@@ -19,7 +19,7 @@
     <t>Work Item</t>
   </si>
   <si>
-    <t>Effort (Hours)</t>
+    <t>Effort Points (Hours)</t>
   </si>
   <si>
     <t>Complexity</t>
@@ -40,31 +40,31 @@
     <t>Past Due - ASAP</t>
   </si>
   <si>
+    <t>BRD</t>
+  </si>
+  <si>
+    <t>Team Review 1</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Milestone 1</t>
+  </si>
+  <si>
+    <t>Team Review 2</t>
+  </si>
+  <si>
+    <t>Milestone 2</t>
+  </si>
+  <si>
+    <t>Team Review 3</t>
+  </si>
+  <si>
     <t>Coding Environment Setup</t>
   </si>
   <si>
     <t xml:space="preserve">Low </t>
-  </si>
-  <si>
-    <t>BRD</t>
-  </si>
-  <si>
-    <t>Team Review 1</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Milestone 1</t>
-  </si>
-  <si>
-    <t>Team Review 2</t>
-  </si>
-  <si>
-    <t>Milestone 2</t>
-  </si>
-  <si>
-    <t>Team Review 3</t>
   </si>
 </sst>
 </file>
@@ -87,7 +87,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +100,12 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -107,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -117,11 +123,20 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -373,16 +388,16 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>15.0</v>
+      <c r="C2" s="3">
+        <v>13.0</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3">
-        <v>45180.0</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="4">
+        <v>45200.0</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -393,17 +408,17 @@
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2">
-        <v>8.0</v>
+      <c r="C3" s="3">
+        <v>55.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3">
-        <v>45193.0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>45194.0</v>
+        <v>7</v>
+      </c>
+      <c r="E3" s="4">
+        <v>45209.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45210.0</v>
       </c>
     </row>
     <row r="4">
@@ -411,19 +426,19 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3">
-        <v>45195.0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>45196.0</v>
+      <c r="E4" s="4">
+        <v>45209.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45210.0</v>
       </c>
     </row>
     <row r="5">
@@ -434,16 +449,16 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>20.0</v>
+        <v>55.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3">
-        <v>45195.0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>45196.0</v>
+        <v>7</v>
+      </c>
+      <c r="E5" s="4">
+        <v>45237.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45238.0</v>
       </c>
     </row>
     <row r="6">
@@ -451,18 +466,18 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2">
-        <v>60.0</v>
+        <v>21.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4">
         <v>45237.0</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <v>45238.0</v>
       </c>
     </row>
@@ -471,19 +486,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2">
-        <v>20.0</v>
+        <v>55.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3">
-        <v>45237.0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>45238.0</v>
+        <v>7</v>
+      </c>
+      <c r="E7" s="4">
+        <v>45270.0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45271.0</v>
       </c>
     </row>
     <row r="8">
@@ -491,18 +506,18 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2">
-        <v>60.0</v>
+        <v>21.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4">
         <v>45270.0</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>45271.0</v>
       </c>
     </row>
@@ -510,20 +525,20 @@
       <c r="A9" s="2">
         <v>8.0</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6">
+        <v>8.0</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3">
-        <v>45270.0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>45271.0</v>
+      <c r="E9" s="7">
+        <v>45193.0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>45194.0</v>
       </c>
     </row>
     <row r="10">

</xml_diff>